<commit_message>
Se hzi la notificacion a un usuario cuando le solicitan un alquiler
</commit_message>
<xml_diff>
--- a/wwwroot/Reportes/ReporteAlquileresAdministrador1002960089.xlsx
+++ b/wwwroot/Reportes/ReporteAlquileresAdministrador1002960089.xlsx
@@ -44,85 +44,85 @@
     <t>GANANCIAS</t>
   </si>
   <si>
-    <t>11/06/2024</t>
-  </si>
-  <si>
-    <t>23/06/2024</t>
+    <t>14/05/2024</t>
+  </si>
+  <si>
+    <t>15/05/2024</t>
   </si>
   <si>
     <t>Diana Gómez</t>
   </si>
   <si>
+    <t>Moto Yamaha FZ</t>
+  </si>
+  <si>
+    <t>Florencia (Caquetá)</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>Gilberto Gómez</t>
+  </si>
+  <si>
+    <t>10/05/2024</t>
+  </si>
+  <si>
+    <t>Mario Gómez</t>
+  </si>
+  <si>
+    <t>Montería (Córdoba)</t>
+  </si>
+  <si>
+    <t>28/04/2024</t>
+  </si>
+  <si>
+    <t>29/04/2024</t>
+  </si>
+  <si>
+    <t>Carro Toyota Land Cruiser Prado</t>
+  </si>
+  <si>
+    <t>Santa Marta (Magdalena)</t>
+  </si>
+  <si>
+    <t>Centro Comercial</t>
+  </si>
+  <si>
+    <t>11/04/2024</t>
+  </si>
+  <si>
+    <t>23/04/2024</t>
+  </si>
+  <si>
     <t>Moto Yamaha XTZ</t>
   </si>
   <si>
     <t>Arauca (Arauca)</t>
   </si>
   <si>
-    <t>Terminal</t>
-  </si>
-  <si>
     <t>Diana Caicedo</t>
   </si>
   <si>
-    <t>10/06/2024</t>
-  </si>
-  <si>
-    <t>15/06/2024</t>
-  </si>
-  <si>
-    <t>Mario Gómez</t>
-  </si>
-  <si>
-    <t>Moto Yamaha FZ</t>
-  </si>
-  <si>
-    <t>Florencia (Caquetá)</t>
-  </si>
-  <si>
-    <t>28/05/2024</t>
-  </si>
-  <si>
-    <t>29/05/2024</t>
-  </si>
-  <si>
-    <t>Carro Toyota Land Cruiser Prado</t>
-  </si>
-  <si>
-    <t>Santa Marta (Magdalena)</t>
-  </si>
-  <si>
-    <t>Centro Comercial</t>
-  </si>
-  <si>
-    <t>20/05/2024</t>
-  </si>
-  <si>
-    <t>21/05/2024</t>
-  </si>
-  <si>
-    <t>Montería (Córdoba)</t>
+    <t>10/04/2024</t>
+  </si>
+  <si>
+    <t>15/04/2024</t>
+  </si>
+  <si>
+    <t>26/03/2024</t>
+  </si>
+  <si>
+    <t>29/03/2024</t>
+  </si>
+  <si>
+    <t>20/03/2024</t>
+  </si>
+  <si>
+    <t>21/03/2024</t>
   </si>
   <si>
     <t>Aeropuerto</t>
-  </si>
-  <si>
-    <t>14/05/2024</t>
-  </si>
-  <si>
-    <t>15/05/2024</t>
-  </si>
-  <si>
-    <t>Gilberto Gómez</t>
-  </si>
-  <si>
-    <t>10/05/2024</t>
-  </si>
-  <si>
-    <t>26/03/2024</t>
-  </si>
-  <si>
-    <t>29/03/2024</t>
   </si>
   <si>
     <t>24/02/2024</t>
@@ -295,10 +295,10 @@
         <v>16</v>
       </c>
       <c r="I2" s="2">
-        <v>285000</v>
+        <v>220000</v>
       </c>
       <c r="J2" s="2">
-        <v>42750</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="3">
@@ -309,16 +309,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
@@ -327,10 +327,10 @@
         <v>16</v>
       </c>
       <c r="I3" s="2">
-        <v>120000</v>
+        <v>370000</v>
       </c>
       <c r="J3" s="2">
-        <v>18000</v>
+        <v>55500</v>
       </c>
     </row>
     <row r="4">
@@ -338,25 +338,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2">
         <v>380000</v>
@@ -370,31 +370,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="I5" s="2">
-        <v>90000</v>
+        <v>285000</v>
       </c>
       <c r="J5" s="2">
-        <v>13500</v>
+        <v>42750</v>
       </c>
     </row>
     <row r="6">
@@ -402,31 +402,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I6" s="2">
-        <v>220000</v>
+        <v>120000</v>
       </c>
       <c r="J6" s="2">
-        <v>33000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="7">
@@ -434,31 +434,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="I7" s="2">
-        <v>370000</v>
+        <v>300000</v>
       </c>
       <c r="J7" s="2">
-        <v>55500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="8">
@@ -466,31 +466,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I8" s="2">
-        <v>300000</v>
+        <v>90000</v>
       </c>
       <c r="J8" s="2">
-        <v>45000</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="9">
@@ -504,19 +504,19 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2">
         <v>400000</v>
@@ -536,19 +536,19 @@
         <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I10" s="2">
         <v>215000</v>
@@ -568,7 +568,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>43</v>
@@ -577,10 +577,10 @@
         <v>44</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I11" s="2">
         <v>390000</v>
@@ -603,16 +603,16 @@
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I12" s="2">
         <v>380000</v>
@@ -632,19 +632,19 @@
         <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I13" s="2">
         <v>725000</v>

</xml_diff>